<commit_message>
-break  AICastAbilityOnPoint if the Loc parameter is null to prevent AI cast spells 0n (0,0)
</commit_message>
<xml_diff>
--- a/translation_Edit.xlsx
+++ b/translation_Edit.xlsx
@@ -2285,19 +2285,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Set Mass Push Lane</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|c009090ffon|r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name=|c009090ff禁用|r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Name=|c009090ff启用|r</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set Mass Push Lane</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>|c009090ffon|r</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name=|c009090ff禁用|r</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2689,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H94" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4971,7 +4971,7 @@
         <v>650</v>
       </c>
       <c r="D100" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E100" t="s">
         <v>645</v>
@@ -4994,7 +4994,7 @@
         <v>652</v>
       </c>
       <c r="D101" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E101" t="s">
         <v>655</v>
@@ -5006,7 +5006,7 @@
         <v>658</v>
       </c>
       <c r="H101" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="102" spans="2:8">
@@ -5029,7 +5029,7 @@
         <v>659</v>
       </c>
       <c r="H102" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>